<commit_message>
system output api is available now
</commit_message>
<xml_diff>
--- a/asset/owners.xlsx
+++ b/asset/owners.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t xml:space="preserve">bankAccountId</t>
   </si>
@@ -28,13 +28,19 @@
     <t xml:space="preserve">type</t>
   </si>
   <si>
+    <t xml:space="preserve">mobileNumber</t>
+  </si>
+  <si>
     <t xml:space="preserve">importer</t>
   </si>
   <si>
+    <t xml:space="preserve">09059242876</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exchanger</t>
+  </si>
+  <si>
     <t xml:space="preserve">exporter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">exchanger</t>
   </si>
 </sst>
 </file>
@@ -141,17 +147,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J6" activeCellId="0" sqref="J6"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -160,7 +166,9 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1"/>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -170,9 +178,11 @@
         <v>1111</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="2"/>
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -182,9 +192,11 @@
         <v>2222</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -194,38 +206,9 @@
         <v>3333</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <v>4444</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
-        <v>5555</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
-        <v>6666</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
-        <v>7777</v>
-      </c>
-      <c r="B8" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
numbers are correct for demo
</commit_message>
<xml_diff>
--- a/asset/owners.xlsx
+++ b/asset/owners.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve">bankAccountId</t>
   </si>
@@ -34,13 +34,19 @@
     <t xml:space="preserve">importer</t>
   </si>
   <si>
-    <t xml:space="preserve">09059242876</t>
+    <t xml:space="preserve">09355772318</t>
   </si>
   <si>
     <t xml:space="preserve">exchanger</t>
   </si>
   <si>
+    <t xml:space="preserve">09027237097</t>
+  </si>
+  <si>
     <t xml:space="preserve">exporter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09123896102</t>
   </si>
 </sst>
 </file>
@@ -50,7 +56,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -76,6 +82,12 @@
       <sz val="10"/>
       <name val="Lohit Devanagari"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val=""/>
+      <family val="1"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -121,7 +133,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -131,6 +143,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -154,10 +170,13 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.33"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -194,8 +213,8 @@
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>4</v>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -206,10 +225,10 @@
         <v>3333</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>